<commit_message>
Add review UI & AddReviewController
</commit_message>
<xml_diff>
--- a/database/Movies.xlsx
+++ b/database/Movies.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohsh\Documents\GitHub\SC2002_Assignment\database\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>Dance all night</t>
   </si>
@@ -171,12 +171,16 @@
   </si>
   <si>
     <t>End of Showing</t>
+  </si>
+  <si>
+    <t>|rating:5review:Great!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -531,289 +535,292 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="37.625" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" customWidth="1"/>
-    <col min="5" max="10" width="8" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.0"/>
+    <col min="2" max="2" customWidth="true" width="23.5"/>
+    <col min="3" max="3" customWidth="true" width="37.625"/>
+    <col min="4" max="4" customWidth="true" style="1" width="8.0"/>
+    <col min="5" max="10" customWidth="true" width="8.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="0">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="0">
         <v>2</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1">
         <v>3</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="0">
         <v>4</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="0">
         <v>5</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="0">
         <v>6</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="0">
         <v>7</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="1">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="1">
         <v>26</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="1">
         <v>30</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="1">
         <v>34</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="1">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" t="s" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="0">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="0">
         <v>0</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>0</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="0">
         <v>0</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0">
         <v>0</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="0">
         <v>0</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="0">
         <v>0</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="D9"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>42</v>
       </c>
+      <c r="B10" t="s" s="0">
+        <v>45</v>
+      </c>
       <c r="D10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="0">
         <v>-1</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="0">
         <v>-1</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>-1</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="0">
         <v>-1</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="0">
         <v>-1</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="0">
         <v>-1</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="0">
         <v>-1</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="0">
         <v>-1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove overall review rating from movie database
</commit_message>
<xml_diff>
--- a/database/Movies.xlsx
+++ b/database/Movies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohsh\Documents\GitHub\SC2002_Assignment\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92DFA1C-F0A0-40A9-9D75-92B5EEC9C7F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB1CE17-1995-40E2-9CA4-2728F01C621A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="8260" xr2:uid="{C9ABD031-C07D-D846-8439-F9FAA3B0C49F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{C9ABD031-C07D-D846-8439-F9FAA3B0C49F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t>Dance all night</t>
   </si>
@@ -165,9 +165,6 @@
   </si>
   <si>
     <t>Movie Review List</t>
-  </si>
-  <si>
-    <t>Overall Reviewer Rating</t>
   </si>
   <si>
     <t>End of Showing</t>
@@ -526,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA69B54E-1050-4942-9338-6C6E0043CE56}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -648,7 +645,7 @@
         <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
@@ -789,36 +786,7 @@
         <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11">
-        <v>-1</v>
-      </c>
-      <c r="C11">
-        <v>-1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>-1</v>
-      </c>
-      <c r="E11">
-        <v>-1</v>
-      </c>
-      <c r="F11">
-        <v>-1</v>
-      </c>
-      <c r="G11">
-        <v>-1</v>
-      </c>
-      <c r="H11">
-        <v>-1</v>
-      </c>
-      <c r="I11">
-        <v>-1</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor fix and enhancement
</commit_message>
<xml_diff>
--- a/database/Movies.xlsx
+++ b/database/Movies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SC2002_Assignment\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D05B860-346E-4602-A261-5CF1D357E38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DB2CD3-1EFE-42BE-85A6-E23A6E5AFC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{C9ABD031-C07D-D846-8439-F9FAA3B0C49F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>Dance all night</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Test Movie</t>
   </si>
   <si>
-    <t>Coffee Movie</t>
-  </si>
-  <si>
     <t>2012 American superhero film based on the Marvel Comics superhero team of the same name.</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>Movie about testing</t>
   </si>
   <si>
-    <t>Movie about coffee</t>
-  </si>
-  <si>
     <t>Now Showing</t>
   </si>
   <si>
@@ -168,6 +162,24 @@
   </si>
   <si>
     <t>End of Showing</t>
+  </si>
+  <si>
+    <t>InsertTest</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>IT,TE</t>
+  </si>
+  <si>
+    <t>UpdateTest</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>UT,TU UT</t>
   </si>
 </sst>
 </file>
@@ -203,9 +215,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,267 +537,300 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA69B54E-1050-4942-9338-6C6E0043CE56}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" customWidth="1"/>
-    <col min="3" max="3" width="37.58203125" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" customWidth="1"/>
-    <col min="5" max="10" width="8" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.58203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="2" customWidth="1"/>
+    <col min="5" max="8" width="8" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.58203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="2">
         <v>3</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="1">
         <v>4</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="1">
         <v>5</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="1">
         <v>6</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="1">
         <v>7</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="62" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="1">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="B9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="C9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B9" t="s">
+      <c r="I9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fill up databases + fix booking dates duplicates
</commit_message>
<xml_diff>
--- a/database/Movies.xlsx
+++ b/database/Movies.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SC2002_Assignment\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohsh\Documents\GitHub\SC2002_Assignment\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DB2CD3-1EFE-42BE-85A6-E23A6E5AFC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EE6EAF-7831-4142-9D06-1D103B08BB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{C9ABD031-C07D-D846-8439-F9FAA3B0C49F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C9ABD031-C07D-D846-8439-F9FAA3B0C49F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
   <si>
     <t>Dance all night</t>
   </si>
@@ -180,12 +180,19 @@
   </si>
   <si>
     <t>UT,TU UT</t>
+  </si>
+  <si>
+    <t>rating:5review:Great Movie!</t>
+  </si>
+  <si>
+    <t>rating:5review:Great Movie!rating:4review:Above average movie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -540,22 +547,22 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.58203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="2" customWidth="1"/>
-    <col min="5" max="8" width="8" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.58203125" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="16.125"/>
+    <col min="2" max="2" customWidth="true" style="1" width="48.625"/>
+    <col min="3" max="3" customWidth="true" style="1" width="37.625"/>
+    <col min="4" max="4" customWidth="true" style="2" width="8.0"/>
+    <col min="5" max="8" customWidth="true" style="1" width="8.0"/>
+    <col min="9" max="9" customWidth="true" style="1" width="13.375"/>
+    <col min="10" max="10" customWidth="true" style="1" width="8.0"/>
+    <col min="11" max="16384" style="1" width="10.625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -587,7 +594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -619,7 +626,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="62" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -651,7 +658,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -683,7 +690,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -715,7 +722,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -747,7 +754,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -779,7 +786,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -811,7 +818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -828,9 +835,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>40</v>
+      </c>
+      <c r="B10" t="s" s="1">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>